<commit_message>
- fixed french translation
</commit_message>
<xml_diff>
--- a/Translation sheets/French.xlsx
+++ b/Translation sheets/French.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="Ten_skoroszyt" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avius\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avius\Desktop\FrenchWorkspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEB2278-95AE-47ED-AD40-538F8E7DB883}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89E32B0-2308-489F-94DE-C9AA377AC809}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" xr2:uid="{CF5D6EBD-60F8-43F9-A1CC-353B0616DA62}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="306">
   <si>
     <t>English</t>
   </si>
@@ -1108,7 +1108,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1392,7 +1392,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1401,20 +1403,48 @@
     </border>
     <border>
       <left/>
-      <right style="slantDashDot">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="slantDashDot">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1474,23 +1504,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1512,38 +1557,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
       <font>
         <b val="0"/>
@@ -1570,14 +1606,111 @@
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="slantDashDot">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1607,53 +1740,39 @@
       </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
+      <border>
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1693,33 +1812,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1755,21 +1847,21 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="1" Name="LanguageData_mapa" RootElement="LanguageData" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+  <Map ID="1" Name="LanguageData" RootElement="LanguageData" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="5" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E789CC9E-5DB3-44D7-B3BF-A6DB59D858C3}" name="Tabela1" displayName="Tabela1" ref="I2:K47" tableType="xml" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3" connectionId="5">
-  <autoFilter ref="I2:K47" xr:uid="{A0B2254A-B303-4A68-A399-8E0730B7AE6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E789CC9E-5DB3-44D7-B3BF-A6DB59D858C3}" name="Tabela1" displayName="Tabela1" ref="I2:K101" tableType="xml" totalsRowShown="0" headerRowDxfId="1" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4" connectionId="5">
+  <autoFilter ref="I2:K101" xr:uid="{A0B2254A-B303-4A68-A399-8E0730B7AE6D}"/>
   <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{1779611B-9B22-4127-BE9E-F389F3211919}" uniqueName="document" name="XML Document" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{1779611B-9B22-4127-BE9E-F389F3211919}" uniqueName="document" name="XML Document" dataDxfId="3">
       <calculatedColumnFormula>H$2</calculatedColumnFormula>
       <xmlColumnPr mapId="1" xpath="/LanguageData/entry/@document" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{6D15A7F2-3C5D-4018-B0D4-6CFA2A30182A}" uniqueName="name" name="XML Name" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{6D15A7F2-3C5D-4018-B0D4-6CFA2A30182A}" uniqueName="name" name="XML Name" dataDxfId="2">
       <calculatedColumnFormula>H3</calculatedColumnFormula>
       <xmlColumnPr mapId="1" xpath="/LanguageData/entry/@name" xmlDataType="string"/>
     </tableColumn>
@@ -2082,15 +2174,15 @@
   <sheetPr codeName="Arkusz1"/>
   <dimension ref="A1:Q321"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="1" customWidth="1"/>
     <col min="2" max="2" width="65.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="68.85546875" style="53" customWidth="1"/>
+    <col min="3" max="3" width="68.85546875" style="37" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.140625" customWidth="1"/>
@@ -2107,32 +2199,32 @@
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="32" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="12"/>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="39"/>
+      <c r="F1" s="42"/>
       <c r="G1" s="11"/>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="40"/>
       <c r="L1" s="20" t="s">
         <v>214</v>
       </c>
       <c r="M1" s="11"/>
     </row>
     <row r="2" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="12"/>
       <c r="E2" s="19" t="s">
         <v>211</v>
@@ -2144,13 +2236,13 @@
       <c r="H2" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="48" t="s">
         <v>213</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="49" t="s">
         <v>216</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="59" t="s">
         <v>217</v>
       </c>
       <c r="L2" s="20" t="s">
@@ -2162,7 +2254,7 @@
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="33" t="s">
         <v>218</v>
       </c>
       <c r="D3" s="12"/>
@@ -2176,15 +2268,15 @@
       <c r="H3" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="I3" s="37" t="str">
+      <c r="I3" s="50" t="str">
         <f t="shared" ref="I3:I47" si="0">H$2</f>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J3" s="36" t="str">
+      <c r="J3" s="51" t="str">
         <f>H3</f>
         <v>PrisonLabor_PrisonerWork</v>
       </c>
-      <c r="K3" s="37" t="str">
+      <c r="K3" s="57" t="str">
         <f>C3&amp;""</f>
         <v>Forcer à travailler</v>
       </c>
@@ -2197,7 +2289,7 @@
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="34" t="s">
         <v>219</v>
       </c>
       <c r="D4" s="12"/>
@@ -2207,16 +2299,16 @@
       <c r="H4" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="I4" s="36" t="str">
+      <c r="I4" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J4" s="36" t="str">
-        <f t="shared" ref="J4:J66" si="1">H4</f>
+      <c r="J4" s="51" t="str">
+        <f t="shared" ref="J4:J47" si="1">H4</f>
         <v>PrisonLabor_WorkAndRecruit</v>
       </c>
-      <c r="K4" s="36" t="str">
-        <f t="shared" ref="K4:K67" si="2">C4&amp;""</f>
+      <c r="K4" s="57" t="str">
+        <f t="shared" ref="K4:K47" si="2">C4&amp;""</f>
         <v>Travailler et recruter</v>
       </c>
       <c r="L4" s="20" t="s">
@@ -2230,7 +2322,7 @@
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="34" t="s">
         <v>220</v>
       </c>
       <c r="D5" s="12"/>
@@ -2240,15 +2332,15 @@
       <c r="H5" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="I5" s="36" t="str">
+      <c r="I5" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J5" s="36" t="str">
+      <c r="J5" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_LazyPrisonerMessage</v>
       </c>
-      <c r="K5" s="36" t="str">
+      <c r="K5" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Votre prisonnier à cessé de travailler !</v>
       </c>
@@ -2261,7 +2353,7 @@
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="34" t="s">
         <v>221</v>
       </c>
       <c r="D6" s="12"/>
@@ -2271,15 +2363,15 @@
       <c r="H6" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="36" t="str">
+      <c r="I6" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J6" s="36" t="str">
+      <c r="J6" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_WardenResponeThreshold</v>
       </c>
-      <c r="K6" s="36" t="str">
+      <c r="K6" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Limite de réponse du gardien</v>
       </c>
@@ -2292,7 +2384,7 @@
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="34" t="s">
         <v>222</v>
       </c>
       <c r="D7" s="12"/>
@@ -2302,15 +2394,15 @@
       <c r="H7" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="I7" s="36" t="str">
+      <c r="I7" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J7" s="36" t="str">
+      <c r="J7" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_StoppingWorkThreshold</v>
       </c>
-      <c r="K7" s="36" t="str">
+      <c r="K7" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Limite d’arrêt de travail</v>
       </c>
@@ -2323,7 +2415,7 @@
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="34" t="s">
         <v>223</v>
       </c>
       <c r="D8" s="12"/>
@@ -2333,15 +2425,15 @@
       <c r="H8" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="I8" s="36" t="str">
+      <c r="I8" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J8" s="36" t="str">
+      <c r="J8" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_WorkTypeDisabled</v>
       </c>
-      <c r="K8" s="36" t="str">
+      <c r="K8" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Type de travail désactivé pour les prisonniers</v>
       </c>
@@ -2356,7 +2448,7 @@
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="34" t="s">
         <v>224</v>
       </c>
       <c r="D9" s="12"/>
@@ -2366,15 +2458,15 @@
       <c r="H9" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I9" s="36" t="str">
+      <c r="I9" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J9" s="36" t="str">
+      <c r="J9" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_ShowNews</v>
       </c>
-      <c r="K9" s="36" t="str">
+      <c r="K9" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Montrer les nouvelles</v>
       </c>
@@ -2389,7 +2481,7 @@
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="34" t="s">
         <v>225</v>
       </c>
       <c r="D10" s="12"/>
@@ -2399,15 +2491,15 @@
       <c r="H10" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="I10" s="36" t="str">
+      <c r="I10" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J10" s="36" t="str">
+      <c r="J10" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_ShowNewsDesc</v>
       </c>
-      <c r="K10" s="36" t="str">
+      <c r="K10" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Montrer les nouvelles à propos des changements du mod quand un prisonnier est détecté</v>
       </c>
@@ -2422,7 +2514,7 @@
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="34" t="s">
         <v>226</v>
       </c>
       <c r="D11" s="12"/>
@@ -2432,15 +2524,15 @@
       <c r="H11" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="I11" s="36" t="str">
+      <c r="I11" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J11" s="36" t="str">
+      <c r="J11" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_DefaultInterMode</v>
       </c>
-      <c r="K11" s="36" t="str">
+      <c r="K11" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Mode d’interaction avec les prisonniers par défaut</v>
       </c>
@@ -2455,7 +2547,7 @@
       <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="34" t="s">
         <v>227</v>
       </c>
       <c r="D12" s="12"/>
@@ -2465,15 +2557,15 @@
       <c r="H12" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="I12" s="36" t="str">
+      <c r="I12" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J12" s="36" t="str">
+      <c r="J12" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_AllowedWorkTypes</v>
       </c>
-      <c r="K12" s="36" t="str">
+      <c r="K12" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Types de travaux autorisés</v>
       </c>
@@ -2488,7 +2580,7 @@
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="34" t="s">
         <v>228</v>
       </c>
       <c r="D13" s="12"/>
@@ -2498,15 +2590,15 @@
       <c r="H13" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="I13" s="36" t="str">
+      <c r="I13" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J13" s="36" t="str">
+      <c r="J13" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_AllowAll</v>
       </c>
-      <c r="K13" s="36" t="str">
+      <c r="K13" s="57" t="str">
         <f t="shared" si="2"/>
         <v>tout autoriser</v>
       </c>
@@ -2521,7 +2613,7 @@
       <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="34" t="s">
         <v>229</v>
       </c>
       <c r="D14" s="12"/>
@@ -2531,15 +2623,15 @@
       <c r="H14" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="I14" s="36" t="str">
+      <c r="I14" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J14" s="36" t="str">
+      <c r="J14" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_AllowAllWorktypes</v>
       </c>
-      <c r="K14" s="36" t="str">
+      <c r="K14" s="57" t="str">
         <f t="shared" si="2"/>
         <v>autoriser tout types de travaux</v>
       </c>
@@ -2554,7 +2646,7 @@
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="34" t="s">
         <v>230</v>
       </c>
       <c r="D15" s="12"/>
@@ -2564,15 +2656,15 @@
       <c r="H15" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="I15" s="36" t="str">
+      <c r="I15" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J15" s="36" t="str">
+      <c r="J15" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_AllowedWorktypesL</v>
       </c>
-      <c r="K15" s="36" t="str">
+      <c r="K15" s="57" t="str">
         <f t="shared" si="2"/>
         <v>types de travaux autorisés</v>
       </c>
@@ -2587,7 +2679,7 @@
       <c r="B16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="34" t="s">
         <v>231</v>
       </c>
       <c r="D16" s="12"/>
@@ -2597,15 +2689,15 @@
       <c r="H16" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I16" s="36" t="str">
+      <c r="I16" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J16" s="36" t="str">
+      <c r="J16" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_Browse</v>
       </c>
-      <c r="K16" s="36" t="str">
+      <c r="K16" s="57" t="str">
         <f t="shared" si="2"/>
         <v>rechercher</v>
       </c>
@@ -2620,7 +2712,7 @@
       <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="34" t="s">
         <v>232</v>
       </c>
       <c r="D17" s="12"/>
@@ -2630,15 +2722,15 @@
       <c r="H17" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="I17" s="36" t="str">
+      <c r="I17" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J17" s="36" t="str">
+      <c r="J17" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_MotivationMechanics</v>
       </c>
-      <c r="K17" s="36" t="str">
+      <c r="K17" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Mécanique de motivation</v>
       </c>
@@ -2653,7 +2745,7 @@
       <c r="B18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="34" t="s">
         <v>233</v>
       </c>
       <c r="D18" s="12"/>
@@ -2663,15 +2755,15 @@
       <c r="H18" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="I18" s="36" t="str">
+      <c r="I18" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J18" s="36" t="str">
+      <c r="J18" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_MotivationWarning</v>
       </c>
-      <c r="K18" s="36" t="str">
+      <c r="K18" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Lorsque coché, les prisonniers ont besoin d’être motivés. ATTENTION : Nécessite de recharger la sauvegarde.</v>
       </c>
@@ -2686,7 +2778,7 @@
       <c r="B19" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C19" s="50" t="s">
+      <c r="C19" s="34" t="s">
         <v>234</v>
       </c>
       <c r="D19" s="12"/>
@@ -2696,15 +2788,15 @@
       <c r="H19" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="I19" s="36" t="str">
+      <c r="I19" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J19" s="36" t="str">
+      <c r="J19" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_MotivationIcons</v>
       </c>
-      <c r="K19" s="36" t="str">
+      <c r="K19" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Icônes d’inspiration/motivation</v>
       </c>
@@ -2719,7 +2811,7 @@
       <c r="B20" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C20" s="50" t="s">
+      <c r="C20" s="34" t="s">
         <v>235</v>
       </c>
       <c r="D20" s="12"/>
@@ -2729,15 +2821,15 @@
       <c r="H20" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="I20" s="36" t="str">
+      <c r="I20" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J20" s="36" t="str">
+      <c r="J20" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_MotivationIconsDesc</v>
       </c>
-      <c r="K20" s="36" t="str">
+      <c r="K20" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Lorsque activé, des icônes seront affichés au dessus de la tête des prisonniers. Un icône bleu pour l’inspiration, et un icône vert pour un gain de motivation grâce à d’autres facteurs.</v>
       </c>
@@ -2752,7 +2844,7 @@
       <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="50" t="s">
+      <c r="C21" s="34" t="s">
         <v>236</v>
       </c>
       <c r="D21" s="12"/>
@@ -2762,15 +2854,15 @@
       <c r="H21" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="I21" s="36" t="str">
+      <c r="I21" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J21" s="36" t="str">
+      <c r="J21" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_CanGrowAdvanced</v>
       </c>
-      <c r="K21" s="36" t="str">
+      <c r="K21" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Les prisonniers peuvent cultiver des plantes avancées.</v>
       </c>
@@ -2785,7 +2877,7 @@
       <c r="B22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="34" t="s">
         <v>237</v>
       </c>
       <c r="D22" s="12"/>
@@ -2795,15 +2887,15 @@
       <c r="H22" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I22" s="36" t="str">
+      <c r="I22" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J22" s="36" t="str">
+      <c r="J22" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_CanGrowAdvancedDesc</v>
       </c>
-      <c r="K22" s="36" t="str">
+      <c r="K22" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Lorsque désactivé, les prisonniers pourront uniquement planter et cultiver les plantes qui ne requièrent aucune compétence en agriculture.</v>
       </c>
@@ -2818,7 +2910,7 @@
       <c r="B23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="50" t="s">
+      <c r="C23" s="34" t="s">
         <v>238</v>
       </c>
       <c r="D23" s="12"/>
@@ -2828,15 +2920,15 @@
       <c r="H23" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="I23" s="36" t="str">
+      <c r="I23" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J23" s="36" t="str">
+      <c r="J23" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_RestartInfo</v>
       </c>
-      <c r="K23" s="36" t="str">
+      <c r="K23" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Redémarrez le jeu puis re-sauvegardez votre partie.</v>
       </c>
@@ -2851,7 +2943,7 @@
       <c r="B24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="50" t="s">
+      <c r="C24" s="34" t="s">
         <v>239</v>
       </c>
       <c r="D24" s="12"/>
@@ -2861,15 +2953,15 @@
       <c r="H24" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="I24" s="36" t="str">
+      <c r="I24" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J24" s="36" t="str">
+      <c r="J24" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_RestartInfo2</v>
       </c>
-      <c r="K24" s="36" t="str">
+      <c r="K24" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Après ces étapes vous pourrez sainement désactiver ce mod.</v>
       </c>
@@ -2884,7 +2976,7 @@
       <c r="B25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="50" t="s">
+      <c r="C25" s="34" t="s">
         <v>240</v>
       </c>
       <c r="D25" s="12"/>
@@ -2894,15 +2986,15 @@
       <c r="H25" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="I25" s="36" t="str">
+      <c r="I25" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J25" s="36" t="str">
+      <c r="J25" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_DisableMod</v>
       </c>
-      <c r="K25" s="36" t="str">
+      <c r="K25" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Désactiver le mod.</v>
       </c>
@@ -2917,7 +3009,7 @@
       <c r="B26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="50" t="s">
+      <c r="C26" s="34" t="s">
         <v>241</v>
       </c>
       <c r="D26" s="12"/>
@@ -2927,15 +3019,15 @@
       <c r="H26" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="I26" s="36" t="str">
+      <c r="I26" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J26" s="36" t="str">
+      <c r="J26" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_DisableModDesc</v>
       </c>
-      <c r="K26" s="36" t="str">
+      <c r="K26" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Lorsque activé, les mondes sont sauvegardés et transférés en « mode sûr», et pourront être joués sans mods.</v>
       </c>
@@ -2950,7 +3042,7 @@
       <c r="B27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="50" t="s">
+      <c r="C27" s="34" t="s">
         <v>242</v>
       </c>
       <c r="D27" s="12"/>
@@ -2960,15 +3052,15 @@
       <c r="H27" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="I27" s="36" t="str">
+      <c r="I27" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J27" s="36" t="str">
+      <c r="J27" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_Version</v>
       </c>
-      <c r="K27" s="36" t="str">
+      <c r="K27" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Version :</v>
       </c>
@@ -2983,7 +3075,7 @@
       <c r="B28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="50" t="s">
+      <c r="C28" s="34" t="s">
         <v>243</v>
       </c>
       <c r="D28" s="12"/>
@@ -2993,15 +3085,15 @@
       <c r="H28" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="I28" s="36" t="str">
+      <c r="I28" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J28" s="36" t="str">
+      <c r="J28" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_Difficulty</v>
       </c>
-      <c r="K28" s="36" t="str">
+      <c r="K28" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Difficulté :</v>
       </c>
@@ -3016,7 +3108,7 @@
       <c r="B29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="50" t="s">
+      <c r="C29" s="34" t="s">
         <v>244</v>
       </c>
       <c r="D29" s="12"/>
@@ -3026,15 +3118,15 @@
       <c r="H29" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="I29" s="36" t="str">
+      <c r="I29" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J29" s="36" t="str">
+      <c r="J29" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_Defaults</v>
       </c>
-      <c r="K29" s="36" t="str">
+      <c r="K29" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Défauts</v>
       </c>
@@ -3049,7 +3141,7 @@
       <c r="B30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="50" t="s">
+      <c r="C30" s="34" t="s">
         <v>29</v>
       </c>
       <c r="D30" s="12"/>
@@ -3059,15 +3151,15 @@
       <c r="H30" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="I30" s="36" t="str">
+      <c r="I30" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J30" s="36" t="str">
+      <c r="J30" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_DifficultyNormal</v>
       </c>
-      <c r="K30" s="36" t="str">
+      <c r="K30" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Normal</v>
       </c>
@@ -3082,7 +3174,7 @@
       <c r="B31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="50" t="s">
+      <c r="C31" s="34" t="s">
         <v>245</v>
       </c>
       <c r="D31" s="12"/>
@@ -3092,15 +3184,15 @@
       <c r="H31" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="I31" s="36" t="str">
+      <c r="I31" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J31" s="36" t="str">
+      <c r="J31" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_DifficultyCasual</v>
       </c>
-      <c r="K31" s="36" t="str">
+      <c r="K31" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Occasionnel</v>
       </c>
@@ -3115,7 +3207,7 @@
       <c r="B32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="50" t="s">
+      <c r="C32" s="34" t="s">
         <v>246</v>
       </c>
       <c r="D32" s="12"/>
@@ -3125,15 +3217,15 @@
       <c r="H32" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="I32" s="36" t="str">
+      <c r="I32" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J32" s="36" t="str">
+      <c r="J32" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_DifficultyEasy</v>
       </c>
-      <c r="K32" s="36" t="str">
+      <c r="K32" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Facile</v>
       </c>
@@ -3148,7 +3240,7 @@
       <c r="B33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="50" t="s">
+      <c r="C33" s="34" t="s">
         <v>247</v>
       </c>
       <c r="D33" s="12"/>
@@ -3158,15 +3250,15 @@
       <c r="H33" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="I33" s="36" t="str">
+      <c r="I33" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J33" s="36" t="str">
+      <c r="J33" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_DifficultyPeaceful</v>
       </c>
-      <c r="K33" s="36" t="str">
+      <c r="K33" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Paisible</v>
       </c>
@@ -3181,7 +3273,7 @@
       <c r="B34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="50" t="s">
+      <c r="C34" s="34" t="s">
         <v>248</v>
       </c>
       <c r="D34" s="12"/>
@@ -3191,15 +3283,15 @@
       <c r="H34" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="I34" s="36" t="str">
+      <c r="I34" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J34" s="36" t="str">
+      <c r="J34" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_DifficultyJoke</v>
       </c>
-      <c r="K34" s="36" t="str">
+      <c r="K34" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Une blague</v>
       </c>
@@ -3214,7 +3306,7 @@
       <c r="B35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="50" t="s">
+      <c r="C35" s="34" t="s">
         <v>249</v>
       </c>
       <c r="D35" s="12"/>
@@ -3224,15 +3316,15 @@
       <c r="H35" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="I35" s="36" t="str">
+      <c r="I35" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J35" s="36" t="str">
+      <c r="J35" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_LazyPrisonerAlert</v>
       </c>
-      <c r="K35" s="36" t="str">
+      <c r="K35" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Les prisonniers ne travaillent pas</v>
       </c>
@@ -3247,7 +3339,7 @@
       <c r="B36" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="50" t="s">
+      <c r="C36" s="34" t="s">
         <v>250</v>
       </c>
       <c r="D36" s="12"/>
@@ -3257,15 +3349,15 @@
       <c r="H36" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I36" s="36" t="str">
+      <c r="I36" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J36" s="36" t="str">
+      <c r="J36" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_LazyPrisonerExplanationDef</v>
       </c>
-      <c r="K36" s="36" t="str">
+      <c r="K36" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Les prisonniers sont fainéants. Essayez de les motiver.</v>
       </c>
@@ -3280,7 +3372,7 @@
       <c r="B37" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="50" t="s">
+      <c r="C37" s="34" t="s">
         <v>251</v>
       </c>
       <c r="D37" s="12"/>
@@ -3290,15 +3382,15 @@
       <c r="H37" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="I37" s="36" t="str">
+      <c r="I37" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J37" s="36" t="str">
+      <c r="J37" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_LazyPrisonerExplanation</v>
       </c>
-      <c r="K37" s="36" t="str">
+      <c r="K37" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Ces prisonniers sont fainéants:\n\n{0}\nEssayez de les motiver.</v>
       </c>
@@ -3313,7 +3405,7 @@
       <c r="B38" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="50" t="s">
+      <c r="C38" s="34" t="s">
         <v>252</v>
       </c>
       <c r="D38" s="12"/>
@@ -3323,15 +3415,15 @@
       <c r="H38" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="I38" s="36" t="str">
+      <c r="I38" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J38" s="36" t="str">
+      <c r="J38" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_StarvingPrisonerAlert</v>
       </c>
-      <c r="K38" s="36" t="str">
+      <c r="K38" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Les prisonniers meurent de faim</v>
       </c>
@@ -3346,7 +3438,7 @@
       <c r="B39" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="50" t="s">
+      <c r="C39" s="34" t="s">
         <v>253</v>
       </c>
       <c r="D39" s="12"/>
@@ -3356,15 +3448,15 @@
       <c r="H39" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="I39" s="36" t="str">
+      <c r="I39" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J39" s="36" t="str">
+      <c r="J39" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_StarvingPrisonerExplanationDef</v>
       </c>
-      <c r="K39" s="36" t="str">
+      <c r="K39" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Les prisonniers meurent de faim et ne travaillerons pas.</v>
       </c>
@@ -3379,7 +3471,7 @@
       <c r="B40" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="50" t="s">
+      <c r="C40" s="34" t="s">
         <v>254</v>
       </c>
       <c r="D40" s="12"/>
@@ -3389,15 +3481,15 @@
       <c r="H40" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="I40" s="36" t="str">
+      <c r="I40" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J40" s="36" t="str">
+      <c r="J40" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_StarvingPrionserExplanation</v>
       </c>
-      <c r="K40" s="36" t="str">
+      <c r="K40" s="57" t="str">
         <f t="shared" si="2"/>
         <v>les prisonniers meurent de faim et ne travaillerons pas:\n\n{0}</v>
       </c>
@@ -3412,7 +3504,7 @@
       <c r="B41" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="50" t="s">
+      <c r="C41" s="34" t="s">
         <v>255</v>
       </c>
       <c r="D41" s="12"/>
@@ -3422,15 +3514,15 @@
       <c r="H41" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="I41" s="36" t="str">
+      <c r="I41" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J41" s="36" t="str">
+      <c r="J41" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_LaborArea</v>
       </c>
-      <c r="K41" s="36" t="str">
+      <c r="K41" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Zone de Travail de Prison</v>
       </c>
@@ -3445,7 +3537,7 @@
       <c r="B42" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="50" t="s">
+      <c r="C42" s="34" t="s">
         <v>256</v>
       </c>
       <c r="D42" s="12"/>
@@ -3455,15 +3547,15 @@
       <c r="H42" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="I42" s="36" t="str">
+      <c r="I42" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J42" s="36" t="str">
+      <c r="J42" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_LaborAreaDesc</v>
       </c>
-      <c r="K42" s="36" t="str">
+      <c r="K42" s="57" t="str">
         <f t="shared" si="2"/>
         <v>La Zone de Travail de Prison est une zone où uniquement les prisonniers peuvent travailler. Les colons n’y sont pas autorisés exceptés les gardiens de prison.</v>
       </c>
@@ -3478,7 +3570,7 @@
       <c r="B43" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="50" t="s">
+      <c r="C43" s="34" t="s">
         <v>257</v>
       </c>
       <c r="D43" s="12"/>
@@ -3488,15 +3580,15 @@
       <c r="H43" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="I43" s="36" t="str">
+      <c r="I43" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J43" s="36" t="str">
+      <c r="J43" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_ClearLaborArea</v>
       </c>
-      <c r="K43" s="36" t="str">
+      <c r="K43" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Supprimer la Zone de Travail de Prison</v>
       </c>
@@ -3511,7 +3603,7 @@
       <c r="B44" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="50" t="s">
+      <c r="C44" s="34" t="s">
         <v>258</v>
       </c>
       <c r="D44" s="12"/>
@@ -3521,15 +3613,15 @@
       <c r="H44" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="I44" s="36" t="str">
+      <c r="I44" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J44" s="36" t="str">
+      <c r="J44" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_ExpandLaborArea</v>
       </c>
-      <c r="K44" s="36" t="str">
+      <c r="K44" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Élargir la Zone de Travail de Prison</v>
       </c>
@@ -3544,7 +3636,7 @@
       <c r="B45" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="50" t="s">
+      <c r="C45" s="34" t="s">
         <v>259</v>
       </c>
       <c r="D45" s="12"/>
@@ -3554,15 +3646,15 @@
       <c r="H45" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="I45" s="36" t="str">
+      <c r="I45" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J45" s="36" t="str">
+      <c r="J45" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_ColonistsOnly</v>
       </c>
-      <c r="K45" s="36" t="str">
+      <c r="K45" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Colons seulement</v>
       </c>
@@ -3577,7 +3669,7 @@
       <c r="B46" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="50" t="s">
+      <c r="C46" s="34" t="s">
         <v>260</v>
       </c>
       <c r="D46" s="12"/>
@@ -3587,15 +3679,15 @@
       <c r="H46" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="I46" s="36" t="str">
+      <c r="I46" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J46" s="36" t="str">
+      <c r="J46" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_PrisonersOnly</v>
       </c>
-      <c r="K46" s="36" t="str">
+      <c r="K46" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Prisonniers seulement</v>
       </c>
@@ -3610,7 +3702,7 @@
       <c r="B47" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="51" t="s">
+      <c r="C47" s="35" t="s">
         <v>261</v>
       </c>
       <c r="D47" s="12"/>
@@ -3620,15 +3712,15 @@
       <c r="H47" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="I47" s="36" t="str">
+      <c r="I47" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Keyed\Keys.xml</v>
       </c>
-      <c r="J47" s="36" t="str">
+      <c r="J47" s="51" t="str">
         <f t="shared" si="1"/>
         <v>PrisonLabor_ColonyOnly</v>
       </c>
-      <c r="K47" s="36" t="str">
+      <c r="K47" s="57" t="str">
         <f t="shared" si="2"/>
         <v>Colonie seulement</v>
       </c>
@@ -3637,11 +3729,11 @@
       </c>
     </row>
     <row r="48" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="40" t="s">
+      <c r="A48" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
       <c r="D48" s="12"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
@@ -3649,14 +3741,9 @@
       <c r="H48" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="I48" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="J48" s="35"/>
-      <c r="K48" s="32" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="I48" s="52"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="58"/>
       <c r="L48" s="20" t="s">
         <v>214</v>
       </c>
@@ -3666,7 +3753,7 @@
       <c r="B49" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="49" t="s">
+      <c r="C49" s="33" t="s">
         <v>262</v>
       </c>
       <c r="D49" s="12"/>
@@ -3676,16 +3763,16 @@
       <c r="H49" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="I49" s="28" t="str">
+      <c r="I49" s="54" t="str">
         <f t="shared" ref="I49:I58" si="3">H$48</f>
         <v>DefInjected\ConceptDef\ConceptDef.xml</v>
       </c>
-      <c r="J49" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="J49" s="51" t="str">
+        <f>H49</f>
         <v>PrisonLabor_Indroduction.label</v>
       </c>
-      <c r="K49" s="29" t="str">
-        <f t="shared" si="2"/>
+      <c r="K49" s="57" t="str">
+        <f>C49&amp;""</f>
         <v>Prison labor (Travail de prison)</v>
       </c>
       <c r="L49" s="20" t="s">
@@ -3697,7 +3784,7 @@
       <c r="B50" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="50" t="s">
+      <c r="C50" s="34" t="s">
         <v>263</v>
       </c>
       <c r="D50" s="12"/>
@@ -3707,16 +3794,16 @@
       <c r="H50" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="I50" s="28" t="str">
+      <c r="I50" s="54" t="str">
         <f t="shared" si="3"/>
         <v>DefInjected\ConceptDef\ConceptDef.xml</v>
       </c>
-      <c r="J50" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="J50" s="51" t="str">
+        <f>H50</f>
         <v>PrisonLabor_Indroduction.helpText</v>
       </c>
-      <c r="K50" s="29" t="str">
-        <f t="shared" si="2"/>
+      <c r="K50" s="57" t="str">
+        <f>C50&amp;""</f>
         <v>Vous pouvez forcer les prisonniers à travailler.\n\nPour se faire, vous devez sélectionner l’option « Forcer à travailler » dans l’onglet « Prisonnier »\n\nLes prisonniers travailleront dans les zones autorisées.  Vérifiez que les prisonniers peuvent atteindre leur travail.\n\nIls peuvent uniquement cuisiner, miner, couper des plantes, transporter, nettoyer ou cultiver des plantes.\n\nLes prisonniers refuseront parfois de travailler. Les raisons peuvent êtres différentes. Ils peuvent être blessés, fatigués, pas assez motivés ou avoir faim.\n\nASTUCE: Vous pouvez assigner le travail depuis l’onglet « Travail ».\n\nASTUCE: Si vous mettez une cuisinière dans leur cellule, vérifiez qu’ils peuvent atteindre les ingrédients.\n\nASTUCE: Vous pouvez permettre aux prisonniers de passer les portes en les laissant ouvertes</v>
       </c>
       <c r="L50" s="20" t="s">
@@ -3728,7 +3815,7 @@
       <c r="B51" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="50" t="s">
+      <c r="C51" s="34" t="s">
         <v>264</v>
       </c>
       <c r="D51" s="12"/>
@@ -3738,16 +3825,16 @@
       <c r="H51" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="I51" s="28" t="str">
+      <c r="I51" s="54" t="str">
         <f t="shared" si="3"/>
         <v>DefInjected\ConceptDef\ConceptDef.xml</v>
       </c>
-      <c r="J51" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="J51" s="51" t="str">
+        <f>H51</f>
         <v>PrisonLabor_Motivation.label</v>
       </c>
-      <c r="K51" s="29" t="str">
-        <f t="shared" si="2"/>
+      <c r="K51" s="57" t="str">
+        <f>C51&amp;""</f>
         <v>Motivation des prisonniers</v>
       </c>
       <c r="L51" s="20" t="s">
@@ -3759,7 +3846,7 @@
       <c r="B52" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="50" t="s">
+      <c r="C52" s="34" t="s">
         <v>265</v>
       </c>
       <c r="D52" s="12"/>
@@ -3769,16 +3856,16 @@
       <c r="H52" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="I52" s="28" t="str">
+      <c r="I52" s="54" t="str">
         <f t="shared" si="3"/>
         <v>DefInjected\ConceptDef\ConceptDef.xml</v>
       </c>
-      <c r="J52" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="J52" s="51" t="str">
+        <f>H52</f>
         <v>PrisonLabor_Motivation.helpText</v>
       </c>
-      <c r="K52" s="29" t="str">
-        <f t="shared" si="2"/>
+      <c r="K52" s="57" t="str">
+        <f>C52&amp;""</f>
         <v>Un de vos prisonniers a cessé de travailler.\nIl ne travaillera pas davantage, à moins qu’on ne le motive.\n\nVous pouvez vérifier la motivation dans l’onglet « Besoins ».\n\nVérifiez que vous avez assez de gardiens (vérifiez l’onglet « Travail »), ou mobilisez un de vos colons et ordonnez lui de rester près des prisonniers.\n\nUne motivation basse peut mener à des révoltes.</v>
       </c>
       <c r="L52" s="20" t="s">
@@ -3790,7 +3877,7 @@
       <c r="B53" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="50" t="s">
+      <c r="C53" s="34" t="s">
         <v>266</v>
       </c>
       <c r="D53" s="12"/>
@@ -3800,16 +3887,16 @@
       <c r="H53" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="I53" s="28" t="str">
+      <c r="I53" s="54" t="str">
         <f t="shared" si="3"/>
         <v>DefInjected\ConceptDef\ConceptDef.xml</v>
       </c>
-      <c r="J53" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="J53" s="51" t="str">
+        <f>H53</f>
         <v>PrisonLabor_Growing.label</v>
       </c>
-      <c r="K53" s="29" t="str">
-        <f t="shared" si="2"/>
+      <c r="K53" s="57" t="str">
+        <f>C53&amp;""</f>
         <v>Cultiver via les prisonniers</v>
       </c>
       <c r="L53" s="20" t="s">
@@ -3821,7 +3908,7 @@
       <c r="B54" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C54" s="50" t="s">
+      <c r="C54" s="34" t="s">
         <v>267</v>
       </c>
       <c r="D54" s="12"/>
@@ -3831,16 +3918,16 @@
       <c r="H54" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="I54" s="28" t="str">
+      <c r="I54" s="54" t="str">
         <f t="shared" si="3"/>
         <v>DefInjected\ConceptDef\ConceptDef.xml</v>
       </c>
-      <c r="J54" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="J54" s="51" t="str">
+        <f>H54</f>
         <v>PrisonLabor_Growing.helpText</v>
       </c>
-      <c r="K54" s="29" t="str">
-        <f t="shared" si="2"/>
+      <c r="K54" s="57" t="str">
+        <f>C54&amp;""</f>
         <v>Les prisonniers peuvent seulement cultiver des plantes qui ne requièrent aucune compétence particulière, comme les patates ou le coton. Ils peuvent en revanche récolter tout type de plante qui est sous ordre de récolte.</v>
       </c>
       <c r="L54" s="20" t="s">
@@ -3852,7 +3939,7 @@
       <c r="B55" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="50" t="s">
+      <c r="C55" s="34" t="s">
         <v>268</v>
       </c>
       <c r="D55" s="12"/>
@@ -3862,16 +3949,16 @@
       <c r="H55" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="I55" s="28" t="str">
+      <c r="I55" s="54" t="str">
         <f t="shared" si="3"/>
         <v>DefInjected\ConceptDef\ConceptDef.xml</v>
       </c>
-      <c r="J55" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="J55" s="51" t="str">
+        <f>H55</f>
         <v>PrisonLabor_Management.label</v>
       </c>
-      <c r="K55" s="29" t="str">
-        <f t="shared" si="2"/>
+      <c r="K55" s="57" t="str">
+        <f>C55&amp;""</f>
         <v>Gestion du travail de prison</v>
       </c>
       <c r="L55" s="20" t="s">
@@ -3883,7 +3970,7 @@
       <c r="B56" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C56" s="50" t="s">
+      <c r="C56" s="34" t="s">
         <v>269</v>
       </c>
       <c r="D56" s="12"/>
@@ -3893,16 +3980,16 @@
       <c r="H56" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="I56" s="28" t="str">
+      <c r="I56" s="54" t="str">
         <f t="shared" si="3"/>
         <v>DefInjected\ConceptDef\ConceptDef.xml</v>
       </c>
-      <c r="J56" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="J56" s="51" t="str">
+        <f>H56</f>
         <v>PrisonLabor_Management.helpText</v>
       </c>
-      <c r="K56" s="29" t="str">
-        <f t="shared" si="2"/>
+      <c r="K56" s="57" t="str">
+        <f>C56&amp;""</f>
         <v>Vous pouvez gérer vos travaux de prison de différente manières.\n\nVous pouvez assigner du travail aux prisonniers depuis l’onglet « Travail ».\n\nVous pouvez configurer quand le prisonnier devra travailler, se reposer ou dormir depuis l’onglet « Restriction ».\n\nVous pouvez restreindre un travail en « Prisonniers seulement ».Pour les travaux qui couvrent une zone, vous pouvez créer une « Zone de travail » dans l’onglet « Architect → Ordres ».\nPour les ordres il y a l’option « Prisonniers seulement ».</v>
       </c>
       <c r="L56" s="20" t="s">
@@ -3914,7 +4001,7 @@
       <c r="B57" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="50" t="s">
+      <c r="C57" s="34" t="s">
         <v>270</v>
       </c>
       <c r="D57" s="12"/>
@@ -3924,16 +4011,16 @@
       <c r="H57" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="I57" s="28" t="str">
+      <c r="I57" s="54" t="str">
         <f t="shared" si="3"/>
         <v>DefInjected\ConceptDef\ConceptDef.xml</v>
       </c>
-      <c r="J57" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="J57" s="51" t="str">
+        <f>H57</f>
         <v>PrisonLabor_Timetable.label</v>
       </c>
-      <c r="K57" s="29" t="str">
-        <f t="shared" si="2"/>
+      <c r="K57" s="57" t="str">
+        <f>C57&amp;""</f>
         <v>Restriction du temps des prisonniers</v>
       </c>
       <c r="L57" s="20" t="s">
@@ -3945,7 +4032,7 @@
       <c r="B58" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="51" t="s">
+      <c r="C58" s="35" t="s">
         <v>271</v>
       </c>
       <c r="D58" s="12"/>
@@ -3955,16 +4042,16 @@
       <c r="H58" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="I58" s="28" t="str">
+      <c r="I58" s="54" t="str">
         <f t="shared" si="3"/>
         <v>DefInjected\ConceptDef\ConceptDef.xml</v>
       </c>
-      <c r="J58" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="J58" s="51" t="str">
+        <f>H58</f>
         <v>PrisonLabor_Timetable.helpText</v>
       </c>
-      <c r="K58" s="29" t="str">
-        <f t="shared" si="2"/>
+      <c r="K58" s="57" t="str">
+        <f>C58&amp;""</f>
         <v>Vous pouvez créer des restrictions pour les prisonniers.\n\nLe temps de "Travail" forcera les prisonniers à travailler, même si ils ont faim ou sont fatigués.\n\nLe temps de "Loisir"leur permettra de se reposer de leur travail et de gagner un bonus de motivation.\n\nLe temps pour "Dormir" les forcera à rester dans leur cellule.\n\n"Temps Libre" est l’option par défaut.</v>
       </c>
       <c r="L58" s="20" t="s">
@@ -3972,11 +4059,11 @@
       </c>
     </row>
     <row r="59" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="40" t="s">
+      <c r="A59" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="40"/>
-      <c r="C59" s="40"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="43"/>
       <c r="D59" s="12"/>
       <c r="E59" s="11"/>
       <c r="F59" s="11"/>
@@ -3984,14 +4071,9 @@
       <c r="H59" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="I59" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="J59" s="31"/>
-      <c r="K59" s="32" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="I59" s="54"/>
+      <c r="J59" s="51"/>
+      <c r="K59" s="57"/>
       <c r="L59" s="20" t="s">
         <v>214</v>
       </c>
@@ -4001,7 +4083,7 @@
       <c r="B60" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C60" s="49" t="s">
+      <c r="C60" s="33" t="s">
         <v>59</v>
       </c>
       <c r="D60" s="12"/>
@@ -4011,16 +4093,16 @@
       <c r="H60" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="I60" s="28" t="str">
+      <c r="I60" s="54" t="str">
         <f>H$59</f>
         <v>DefInjected\NeedDef\Needs.xml</v>
       </c>
-      <c r="J60" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="J60" s="51" t="str">
+        <f>H60</f>
         <v>PrisonLabor_Motivation.label</v>
       </c>
-      <c r="K60" s="29" t="str">
-        <f t="shared" si="2"/>
+      <c r="K60" s="57" t="str">
+        <f>C60&amp;""</f>
         <v>Motivation</v>
       </c>
       <c r="L60" s="20" t="s">
@@ -4032,7 +4114,7 @@
       <c r="B61" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C61" s="51" t="s">
+      <c r="C61" s="35" t="s">
         <v>272</v>
       </c>
       <c r="D61" s="12"/>
@@ -4042,16 +4124,16 @@
       <c r="H61" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="I61" s="28" t="str">
+      <c r="I61" s="54" t="str">
         <f>H$59</f>
         <v>DefInjected\NeedDef\Needs.xml</v>
       </c>
-      <c r="J61" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="J61" s="51" t="str">
+        <f>H61</f>
         <v>PrisonLabor_Motivation.description</v>
       </c>
-      <c r="K61" s="29" t="str">
-        <f t="shared" si="2"/>
+      <c r="K61" s="57" t="str">
+        <f>C61&amp;""</f>
         <v>La motivation représente à quel point le prisonnier est motivé pour travailler. La motivation peut être augmentée par les colons qui restent à proximité.</v>
       </c>
       <c r="L61" s="20" t="s">
@@ -4059,11 +4141,11 @@
       </c>
     </row>
     <row r="62" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="40" t="s">
+      <c r="A62" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="B62" s="40"/>
-      <c r="C62" s="40"/>
+      <c r="B62" s="43"/>
+      <c r="C62" s="43"/>
       <c r="D62" s="12"/>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
@@ -4071,12 +4153,15 @@
       <c r="H62" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="I62" s="31" t="s">
+      <c r="I62" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="J62" s="31"/>
-      <c r="K62" s="32" t="str">
-        <f t="shared" si="2"/>
+      <c r="J62" s="51" t="str">
+        <f>H62</f>
+        <v>DefInjected\HediffDef\Hediffs.xml</v>
+      </c>
+      <c r="K62" s="57" t="str">
+        <f>C62&amp;""</f>
         <v/>
       </c>
       <c r="L62" s="20" t="s">
@@ -4088,7 +4173,7 @@
       <c r="B63" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C63" s="49" t="s">
+      <c r="C63" s="33" t="s">
         <v>273</v>
       </c>
       <c r="D63" s="12"/>
@@ -4098,16 +4183,16 @@
       <c r="H63" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="I63" s="28" t="str">
+      <c r="I63" s="54" t="str">
         <f>H$62</f>
         <v>DefInjected\HediffDef\Hediffs.xml</v>
       </c>
-      <c r="J63" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="J63" s="51" t="str">
+        <f>H63</f>
         <v>PrisonLabor_PrisonerChains.stages.0.label</v>
       </c>
-      <c r="K63" s="29" t="str">
-        <f t="shared" si="2"/>
+      <c r="K63" s="57" t="str">
+        <f>C63&amp;""</f>
         <v>non actif</v>
       </c>
       <c r="L63" s="20" t="s">
@@ -4119,7 +4204,7 @@
       <c r="B64" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C64" s="50" t="s">
+      <c r="C64" s="34" t="s">
         <v>274</v>
       </c>
       <c r="D64" s="12"/>
@@ -4129,16 +4214,16 @@
       <c r="H64" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="I64" s="28" t="str">
+      <c r="I64" s="54" t="str">
         <f>H$62</f>
         <v>DefInjected\HediffDef\Hediffs.xml</v>
       </c>
-      <c r="J64" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="J64" s="51" t="str">
+        <f>H64</f>
         <v>PrisonLabor_PrisonerChains.stages.1.label</v>
       </c>
-      <c r="K64" s="29" t="str">
-        <f t="shared" si="2"/>
+      <c r="K64" s="57" t="str">
+        <f>C64&amp;""</f>
         <v>chaines de prissonier</v>
       </c>
       <c r="L64" s="20" t="s">
@@ -4150,7 +4235,7 @@
       <c r="B65" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="50" t="s">
+      <c r="C65" s="34" t="s">
         <v>275</v>
       </c>
       <c r="D65" s="12"/>
@@ -4158,15 +4243,9 @@
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
       <c r="H65" s="13"/>
-      <c r="I65" s="28"/>
-      <c r="J65" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K65" s="29" t="str">
-        <f t="shared" si="2"/>
-        <v>motivé</v>
-      </c>
+      <c r="I65" s="54"/>
+      <c r="J65" s="51"/>
+      <c r="K65" s="57"/>
       <c r="L65" s="20" t="s">
         <v>214</v>
       </c>
@@ -4176,7 +4255,7 @@
       <c r="B66" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="51" t="s">
+      <c r="C66" s="35" t="s">
         <v>276</v>
       </c>
       <c r="D66" s="12"/>
@@ -4184,25 +4263,19 @@
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
       <c r="H66" s="13"/>
-      <c r="I66" s="28"/>
-      <c r="J66" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K66" s="29" t="str">
-        <f t="shared" si="2"/>
-        <v>inspiré</v>
-      </c>
+      <c r="I66" s="54"/>
+      <c r="J66" s="51"/>
+      <c r="K66" s="57"/>
       <c r="L66" s="20" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="40" t="s">
+      <c r="A67" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="B67" s="40"/>
-      <c r="C67" s="40"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="43"/>
       <c r="D67" s="12"/>
       <c r="E67" s="11"/>
       <c r="F67" s="11"/>
@@ -4210,12 +4283,12 @@
       <c r="H67" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="I67" s="31" t="s">
+      <c r="I67" s="52" t="s">
         <v>159</v>
       </c>
-      <c r="J67" s="31"/>
-      <c r="K67" s="32" t="str">
-        <f t="shared" si="2"/>
+      <c r="J67" s="53"/>
+      <c r="K67" s="58" t="str">
+        <f>C67&amp;""</f>
         <v/>
       </c>
       <c r="L67" s="20" t="s">
@@ -4227,7 +4300,7 @@
       <c r="B68" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="49" t="s">
+      <c r="C68" s="33" t="s">
         <v>277</v>
       </c>
       <c r="D68" s="12"/>
@@ -4237,16 +4310,16 @@
       <c r="H68" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="I68" s="28" t="str">
+      <c r="I68" s="54" t="str">
         <f>H$67</f>
         <v>DefInjected\IncidentDef\Incidents.xml</v>
       </c>
-      <c r="J68" s="28" t="str">
+      <c r="J68" s="51" t="str">
         <f t="shared" ref="J68:J101" si="4">H68</f>
         <v>PrisonLabor_Revolt.label</v>
       </c>
-      <c r="K68" s="29" t="str">
-        <f t="shared" ref="K68:K107" si="5">C68&amp;""</f>
+      <c r="K68" s="57" t="str">
+        <f t="shared" ref="K68:K102" si="5">C68&amp;""</f>
         <v>révolte</v>
       </c>
       <c r="L68" s="20" t="s">
@@ -4258,7 +4331,7 @@
       <c r="B69" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C69" s="50" t="s">
+      <c r="C69" s="34" t="s">
         <v>278</v>
       </c>
       <c r="D69" s="12"/>
@@ -4268,15 +4341,15 @@
       <c r="H69" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="I69" s="28" t="str">
+      <c r="I69" s="54" t="str">
         <f>H$67</f>
         <v>DefInjected\IncidentDef\Incidents.xml</v>
       </c>
-      <c r="J69" s="28" t="str">
+      <c r="J69" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_Revolt.letterLabel</v>
       </c>
-      <c r="K69" s="29" t="str">
+      <c r="K69" s="57" t="str">
         <f t="shared" si="5"/>
         <v>Révolte</v>
       </c>
@@ -4289,7 +4362,7 @@
       <c r="B70" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="51" t="s">
+      <c r="C70" s="35" t="s">
         <v>279</v>
       </c>
       <c r="D70" s="12"/>
@@ -4297,27 +4370,21 @@
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
       <c r="H70" s="13"/>
-      <c r="I70" s="28" t="s">
+      <c r="I70" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="J70" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K70" s="29" t="str">
-        <f t="shared" si="5"/>
-        <v>Une révolte peut être enclenchée par {0}. Les prisonniers se son unis sous la faction {1}, et ont commencés à se révolter avec des armes faites-main.</v>
-      </c>
+      <c r="J70" s="51"/>
+      <c r="K70" s="57"/>
       <c r="L70" s="20" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="40" t="s">
+      <c r="A71" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="B71" s="40"/>
-      <c r="C71" s="40"/>
+      <c r="B71" s="43"/>
+      <c r="C71" s="43"/>
       <c r="D71" s="12"/>
       <c r="E71" s="11"/>
       <c r="F71" s="11"/>
@@ -4325,14 +4392,9 @@
       <c r="H71" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="I71" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="J71" s="31"/>
-      <c r="K71" s="32" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="I71" s="52"/>
+      <c r="J71" s="53"/>
+      <c r="K71" s="58"/>
       <c r="L71" s="20" t="s">
         <v>214</v>
       </c>
@@ -4342,7 +4404,7 @@
       <c r="B72" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C72" s="49" t="s">
+      <c r="C72" s="33" t="s">
         <v>280</v>
       </c>
       <c r="D72" s="12"/>
@@ -4352,15 +4414,15 @@
       <c r="H72" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="I72" s="28" t="str">
+      <c r="I72" s="54" t="str">
         <f>H$71</f>
         <v>DefInjected\JobDef\JobDef.xml</v>
       </c>
-      <c r="J72" s="28" t="str">
+      <c r="J72" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_PrisonerSupervise.reportString</v>
       </c>
-      <c r="K72" s="29" t="str">
+      <c r="K72" s="57" t="str">
         <f t="shared" si="5"/>
         <v>surveille le prisonnier TargetA.</v>
       </c>
@@ -4375,7 +4437,7 @@
       <c r="B73" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C73" s="50" t="s">
+      <c r="C73" s="34" t="s">
         <v>281</v>
       </c>
       <c r="D73" s="12"/>
@@ -4385,15 +4447,15 @@
       <c r="H73" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="I73" s="28" t="str">
+      <c r="I73" s="54" t="str">
         <f>H$71</f>
         <v>DefInjected\JobDef\JobDef.xml</v>
       </c>
-      <c r="J73" s="28" t="str">
+      <c r="J73" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_DeliverFood_Tweak.reportString</v>
       </c>
-      <c r="K73" s="29" t="str">
+      <c r="K73" s="57" t="str">
         <f t="shared" si="5"/>
         <v>nourrit TargetB avec TargetA</v>
       </c>
@@ -4408,7 +4470,7 @@
       <c r="B74" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C74" s="50" t="s">
+      <c r="C74" s="34" t="s">
         <v>282</v>
       </c>
       <c r="D74" s="12"/>
@@ -4418,15 +4480,15 @@
       <c r="H74" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="I74" s="28" t="str">
+      <c r="I74" s="54" t="str">
         <f>H$71</f>
         <v>DefInjected\JobDef\JobDef.xml</v>
       </c>
-      <c r="J74" s="28" t="str">
+      <c r="J74" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_Mine_Tweak.reportString</v>
       </c>
-      <c r="K74" s="29" t="str">
+      <c r="K74" s="57" t="str">
         <f t="shared" si="5"/>
         <v>creuse TargetA</v>
       </c>
@@ -4441,7 +4503,7 @@
       <c r="B75" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C75" s="50" t="s">
+      <c r="C75" s="34" t="s">
         <v>283</v>
       </c>
       <c r="D75" s="12"/>
@@ -4451,15 +4513,15 @@
       <c r="H75" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="I75" s="28" t="str">
+      <c r="I75" s="54" t="str">
         <f>H$71</f>
         <v>DefInjected\JobDef\JobDef.xml</v>
       </c>
-      <c r="J75" s="28" t="str">
+      <c r="J75" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_Harvest_Tweak.reportString</v>
       </c>
-      <c r="K75" s="29" t="str">
+      <c r="K75" s="57" t="str">
         <f t="shared" si="5"/>
         <v>récolte TargetA</v>
       </c>
@@ -4474,7 +4536,7 @@
       <c r="B76" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C76" s="51" t="s">
+      <c r="C76" s="35" t="s">
         <v>284</v>
       </c>
       <c r="D76" s="12"/>
@@ -4484,15 +4546,15 @@
       <c r="H76" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="I76" s="28" t="str">
+      <c r="I76" s="54" t="str">
         <f>H$71</f>
         <v>DefInjected\JobDef\JobDef.xml</v>
       </c>
-      <c r="J76" s="28" t="str">
+      <c r="J76" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_CutPlant_Tweak.reportString</v>
       </c>
-      <c r="K76" s="29" t="str">
+      <c r="K76" s="57" t="str">
         <f t="shared" si="5"/>
         <v>coupe TargetA</v>
       </c>
@@ -4501,11 +4563,11 @@
       </c>
     </row>
     <row r="77" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="40" t="s">
+      <c r="A77" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="B77" s="40"/>
-      <c r="C77" s="40"/>
+      <c r="B77" s="43"/>
+      <c r="C77" s="43"/>
       <c r="D77" s="12"/>
       <c r="E77" s="11"/>
       <c r="F77" s="11"/>
@@ -4513,14 +4575,9 @@
       <c r="H77" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="I77" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="J77" s="31"/>
-      <c r="K77" s="32" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="I77" s="52"/>
+      <c r="J77" s="53"/>
+      <c r="K77" s="58"/>
       <c r="L77" s="20" t="s">
         <v>214</v>
       </c>
@@ -4530,7 +4587,7 @@
       <c r="B78" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C78" s="49" t="s">
+      <c r="C78" s="33" t="s">
         <v>285</v>
       </c>
       <c r="D78" s="12"/>
@@ -4540,15 +4597,15 @@
       <c r="H78" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I78" s="28" t="str">
+      <c r="I78" s="54" t="str">
         <f t="shared" ref="I78:I98" si="6">H$77</f>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J78" s="28" t="str">
+      <c r="J78" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_SupervisePrisonLabor.label</v>
       </c>
-      <c r="K78" s="29" t="str">
+      <c r="K78" s="57" t="str">
         <f t="shared" si="5"/>
         <v>surveiller le prisonnier</v>
       </c>
@@ -4561,7 +4618,7 @@
       <c r="B79" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C79" s="50" t="s">
+      <c r="C79" s="34" t="s">
         <v>285</v>
       </c>
       <c r="D79" s="12"/>
@@ -4571,15 +4628,15 @@
       <c r="H79" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="I79" s="28" t="str">
+      <c r="I79" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J79" s="28" t="str">
+      <c r="J79" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_SupervisePrisonLabor.verb</v>
       </c>
-      <c r="K79" s="29" t="str">
+      <c r="K79" s="57" t="str">
         <f t="shared" si="5"/>
         <v>surveiller le prisonnier</v>
       </c>
@@ -4592,7 +4649,7 @@
       <c r="B80" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C80" s="50" t="s">
+      <c r="C80" s="34" t="s">
         <v>286</v>
       </c>
       <c r="D80" s="12"/>
@@ -4602,15 +4659,15 @@
       <c r="H80" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="I80" s="28" t="str">
+      <c r="I80" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J80" s="28" t="str">
+      <c r="J80" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_SupervisePrisonLabor.gerund</v>
       </c>
-      <c r="K80" s="29" t="str">
+      <c r="K80" s="57" t="str">
         <f t="shared" si="5"/>
         <v>surveille le prisonnier</v>
       </c>
@@ -4625,7 +4682,7 @@
       <c r="B81" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C81" s="50" t="s">
+      <c r="C81" s="34" t="s">
         <v>287</v>
       </c>
       <c r="D81" s="12"/>
@@ -4635,15 +4692,15 @@
       <c r="H81" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="I81" s="28" t="str">
+      <c r="I81" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J81" s="28" t="str">
+      <c r="J81" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_DeliverFoodToPrisoner_Tweak.label</v>
       </c>
-      <c r="K81" s="29" t="str">
+      <c r="K81" s="57" t="str">
         <f t="shared" si="5"/>
         <v>apporter de la nourriture aux prisonniers</v>
       </c>
@@ -4658,7 +4715,7 @@
       <c r="B82" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C82" s="50" t="s">
+      <c r="C82" s="34" t="s">
         <v>288</v>
       </c>
       <c r="D82" s="12"/>
@@ -4668,15 +4725,15 @@
       <c r="H82" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="I82" s="28" t="str">
+      <c r="I82" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J82" s="28" t="str">
+      <c r="J82" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_DeliverFoodToPrisoner_Tweak.verb</v>
       </c>
-      <c r="K82" s="29" t="str">
+      <c r="K82" s="57" t="str">
         <f t="shared" si="5"/>
         <v>apporter de la nourriture pour</v>
       </c>
@@ -4691,7 +4748,7 @@
       <c r="B83" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C83" s="50" t="s">
+      <c r="C83" s="34" t="s">
         <v>289</v>
       </c>
       <c r="D83" s="12"/>
@@ -4701,15 +4758,15 @@
       <c r="H83" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="I83" s="28" t="str">
+      <c r="I83" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J83" s="28" t="str">
+      <c r="J83" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_DeliverFoodToPrisoner_Tweak.gerund</v>
       </c>
-      <c r="K83" s="29" t="str">
+      <c r="K83" s="57" t="str">
         <f t="shared" si="5"/>
         <v>apporte de la nourriture pour</v>
       </c>
@@ -4724,7 +4781,7 @@
       <c r="B84" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C84" s="50" t="s">
+      <c r="C84" s="34" t="s">
         <v>290</v>
       </c>
       <c r="D84" s="12"/>
@@ -4734,15 +4791,15 @@
       <c r="H84" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="I84" s="28" t="str">
+      <c r="I84" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J84" s="28" t="str">
+      <c r="J84" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_Mine_Tweak.label</v>
       </c>
-      <c r="K84" s="29" t="str">
+      <c r="K84" s="57" t="str">
         <f t="shared" si="5"/>
         <v>miner</v>
       </c>
@@ -4757,7 +4814,7 @@
       <c r="B85" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C85" s="50" t="s">
+      <c r="C85" s="34" t="s">
         <v>290</v>
       </c>
       <c r="D85" s="12"/>
@@ -4767,15 +4824,15 @@
       <c r="H85" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="I85" s="28" t="str">
+      <c r="I85" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J85" s="28" t="str">
+      <c r="J85" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_Mine_Tweak.verb</v>
       </c>
-      <c r="K85" s="29" t="str">
+      <c r="K85" s="57" t="str">
         <f t="shared" si="5"/>
         <v>miner</v>
       </c>
@@ -4790,7 +4847,7 @@
       <c r="B86" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C86" s="50" t="s">
+      <c r="C86" s="34" t="s">
         <v>81</v>
       </c>
       <c r="D86" s="12"/>
@@ -4800,15 +4857,15 @@
       <c r="H86" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="I86" s="28" t="str">
+      <c r="I86" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J86" s="28" t="str">
+      <c r="J86" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_Mine_Tweak.gerund</v>
       </c>
-      <c r="K86" s="29" t="str">
+      <c r="K86" s="57" t="str">
         <f t="shared" si="5"/>
         <v>mine</v>
       </c>
@@ -4823,7 +4880,7 @@
       <c r="B87" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C87" s="50" t="s">
+      <c r="C87" s="34" t="s">
         <v>291</v>
       </c>
       <c r="D87" s="12"/>
@@ -4833,15 +4890,15 @@
       <c r="H87" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="I87" s="28" t="str">
+      <c r="I87" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J87" s="28" t="str">
+      <c r="J87" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_PlantsCut_Tweak.label</v>
       </c>
-      <c r="K87" s="29" t="str">
+      <c r="K87" s="57" t="str">
         <f t="shared" si="5"/>
         <v>couper les plantes</v>
       </c>
@@ -4856,7 +4913,7 @@
       <c r="B88" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C88" s="50" t="s">
+      <c r="C88" s="34" t="s">
         <v>292</v>
       </c>
       <c r="D88" s="12"/>
@@ -4866,15 +4923,15 @@
       <c r="H88" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="I88" s="28" t="str">
+      <c r="I88" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J88" s="28" t="str">
+      <c r="J88" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_PlantsCut_Tweak.verb</v>
       </c>
-      <c r="K88" s="29" t="str">
+      <c r="K88" s="57" t="str">
         <f t="shared" si="5"/>
         <v>couper</v>
       </c>
@@ -4889,7 +4946,7 @@
       <c r="B89" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C89" s="50" t="s">
+      <c r="C89" s="34" t="s">
         <v>293</v>
       </c>
       <c r="D89" s="12"/>
@@ -4899,15 +4956,15 @@
       <c r="H89" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="I89" s="28" t="str">
+      <c r="I89" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J89" s="28" t="str">
+      <c r="J89" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_PlantsCut_Tweak.gerund</v>
       </c>
-      <c r="K89" s="29" t="str">
+      <c r="K89" s="57" t="str">
         <f t="shared" si="5"/>
         <v>coupe</v>
       </c>
@@ -4922,7 +4979,7 @@
       <c r="B90" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C90" s="50" t="s">
+      <c r="C90" s="34" t="s">
         <v>294</v>
       </c>
       <c r="D90" s="12"/>
@@ -4932,15 +4989,15 @@
       <c r="H90" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="I90" s="28" t="str">
+      <c r="I90" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J90" s="28" t="str">
+      <c r="J90" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_GrowerHarvest_Tweak.label</v>
       </c>
-      <c r="K90" s="29" t="str">
+      <c r="K90" s="57" t="str">
         <f t="shared" si="5"/>
         <v>récolter les plantes</v>
       </c>
@@ -4955,7 +5012,7 @@
       <c r="B91" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C91" s="50" t="s">
+      <c r="C91" s="34" t="s">
         <v>295</v>
       </c>
       <c r="D91" s="12"/>
@@ -4965,15 +5022,15 @@
       <c r="H91" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="I91" s="28" t="str">
+      <c r="I91" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J91" s="28" t="str">
+      <c r="J91" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_GrowerHarvest_Tweak.verb</v>
       </c>
-      <c r="K91" s="29" t="str">
+      <c r="K91" s="57" t="str">
         <f t="shared" si="5"/>
         <v>récolter</v>
       </c>
@@ -4988,7 +5045,7 @@
       <c r="B92" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C92" s="50" t="s">
+      <c r="C92" s="34" t="s">
         <v>296</v>
       </c>
       <c r="D92" s="12"/>
@@ -4998,15 +5055,15 @@
       <c r="H92" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="I92" s="28" t="str">
+      <c r="I92" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J92" s="28" t="str">
+      <c r="J92" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_GrowerHarvest_Tweak.gerund</v>
       </c>
-      <c r="K92" s="29" t="str">
+      <c r="K92" s="57" t="str">
         <f t="shared" si="5"/>
         <v>récolte</v>
       </c>
@@ -5021,7 +5078,7 @@
       <c r="B93" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C93" s="50" t="s">
+      <c r="C93" s="34" t="s">
         <v>297</v>
       </c>
       <c r="D93" s="12"/>
@@ -5031,15 +5088,15 @@
       <c r="H93" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="I93" s="28" t="str">
+      <c r="I93" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J93" s="28" t="str">
+      <c r="J93" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_GrowerSow_Tweak.label</v>
       </c>
-      <c r="K93" s="29" t="str">
+      <c r="K93" s="57" t="str">
         <f t="shared" si="5"/>
         <v>semer les plantes</v>
       </c>
@@ -5054,7 +5111,7 @@
       <c r="B94" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C94" s="50" t="s">
+      <c r="C94" s="34" t="s">
         <v>298</v>
       </c>
       <c r="D94" s="12"/>
@@ -5064,15 +5121,15 @@
       <c r="H94" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="I94" s="28" t="str">
+      <c r="I94" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J94" s="28" t="str">
+      <c r="J94" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_GrowerSow_Tweak.verb</v>
       </c>
-      <c r="K94" s="29" t="str">
+      <c r="K94" s="57" t="str">
         <f t="shared" si="5"/>
         <v>semer</v>
       </c>
@@ -5087,7 +5144,7 @@
       <c r="B95" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C95" s="50" t="s">
+      <c r="C95" s="34" t="s">
         <v>299</v>
       </c>
       <c r="D95" s="12"/>
@@ -5097,15 +5154,15 @@
       <c r="H95" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="I95" s="28" t="str">
+      <c r="I95" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J95" s="28" t="str">
+      <c r="J95" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_GrowerSow_Tweak.gerund</v>
       </c>
-      <c r="K95" s="29" t="str">
+      <c r="K95" s="57" t="str">
         <f t="shared" si="5"/>
         <v>sème</v>
       </c>
@@ -5120,7 +5177,7 @@
       <c r="B96" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C96" s="50" t="s">
+      <c r="C96" s="34" t="s">
         <v>300</v>
       </c>
       <c r="D96" s="12"/>
@@ -5130,15 +5187,15 @@
       <c r="H96" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="I96" s="28" t="str">
+      <c r="I96" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J96" s="28" t="str">
+      <c r="J96" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_CleanFilth_Tweak.label</v>
       </c>
-      <c r="K96" s="29" t="str">
+      <c r="K96" s="57" t="str">
         <f t="shared" si="5"/>
         <v>nettoyer la saleté</v>
       </c>
@@ -5153,7 +5210,7 @@
       <c r="B97" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C97" s="50" t="s">
+      <c r="C97" s="34" t="s">
         <v>301</v>
       </c>
       <c r="D97" s="12"/>
@@ -5163,15 +5220,15 @@
       <c r="H97" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="I97" s="28" t="str">
+      <c r="I97" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J97" s="28" t="str">
+      <c r="J97" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_CleanFilth_Tweak.verb</v>
       </c>
-      <c r="K97" s="29" t="str">
+      <c r="K97" s="57" t="str">
         <f t="shared" si="5"/>
         <v>nettoyer</v>
       </c>
@@ -5186,7 +5243,7 @@
       <c r="B98" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C98" s="51" t="s">
+      <c r="C98" s="35" t="s">
         <v>302</v>
       </c>
       <c r="D98" s="12"/>
@@ -5196,15 +5253,15 @@
       <c r="H98" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="I98" s="28" t="str">
+      <c r="I98" s="54" t="str">
         <f t="shared" si="6"/>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
-      <c r="J98" s="28" t="str">
+      <c r="J98" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_CleanFilth_Tweak.gerund</v>
       </c>
-      <c r="K98" s="29" t="str">
+      <c r="K98" s="57" t="str">
         <f t="shared" si="5"/>
         <v>nettoie</v>
       </c>
@@ -5213,11 +5270,11 @@
       </c>
     </row>
     <row r="99" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="42" t="s">
+      <c r="A99" s="45" t="s">
         <v>208</v>
       </c>
-      <c r="B99" s="43"/>
-      <c r="C99" s="44"/>
+      <c r="B99" s="46"/>
+      <c r="C99" s="47"/>
       <c r="D99" s="12"/>
       <c r="E99" s="11"/>
       <c r="F99" s="11"/>
@@ -5225,14 +5282,9 @@
       <c r="H99" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="I99" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="J99" s="31"/>
-      <c r="K99" s="32" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="I99" s="52"/>
+      <c r="J99" s="53"/>
+      <c r="K99" s="58"/>
       <c r="L99" s="20" t="s">
         <v>214</v>
       </c>
@@ -5242,7 +5294,7 @@
       <c r="B100" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C100" s="49" t="str">
+      <c r="C100" s="33" t="str">
         <f>C3&amp;""</f>
         <v>Forcer à travailler</v>
       </c>
@@ -5253,15 +5305,15 @@
       <c r="H100" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="I100" s="28" t="str">
+      <c r="I100" s="54" t="str">
         <f>H$99</f>
         <v>DefInjected\InteractionDefs\PrisonerInteractionModeDef.xml</v>
       </c>
-      <c r="J100" s="28" t="str">
+      <c r="J100" s="51" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_workOption.label</v>
       </c>
-      <c r="K100" s="29" t="str">
+      <c r="K100" s="57" t="str">
         <f t="shared" si="5"/>
         <v>Forcer à travailler</v>
       </c>
@@ -5274,7 +5326,7 @@
       <c r="B101" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C101" s="52" t="str">
+      <c r="C101" s="36" t="str">
         <f>C4&amp;""</f>
         <v>Travailler et recruter</v>
       </c>
@@ -5285,15 +5337,15 @@
       <c r="H101" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="I101" s="28" t="str">
-        <f>H$100</f>
-        <v>PrisonLabor_workOption.label</v>
-      </c>
-      <c r="J101" s="28" t="str">
+      <c r="I101" s="55" t="str">
+        <f>H$99</f>
+        <v>DefInjected\InteractionDefs\PrisonerInteractionModeDef.xml</v>
+      </c>
+      <c r="J101" s="56" t="str">
         <f t="shared" si="4"/>
         <v>PrisonLabor_workAndRecruitOption.label</v>
       </c>
-      <c r="K101" s="29" t="str">
+      <c r="K101" s="57" t="str">
         <f t="shared" si="5"/>
         <v>Travailler et recruter</v>
       </c>
@@ -5302,21 +5354,21 @@
       </c>
     </row>
     <row r="102" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="40" t="s">
+      <c r="A102" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="B102" s="40"/>
-      <c r="C102" s="40"/>
+      <c r="B102" s="43"/>
+      <c r="C102" s="43"/>
       <c r="D102" s="12"/>
       <c r="E102" s="11"/>
       <c r="F102" s="11"/>
       <c r="G102" s="11"/>
       <c r="H102" s="23"/>
-      <c r="I102" s="31" t="s">
+      <c r="I102" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="J102" s="31"/>
-      <c r="K102" s="32" t="str">
+      <c r="J102" s="30"/>
+      <c r="K102" s="31" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
@@ -5331,7 +5383,7 @@
       <c r="B103" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C103" s="49" t="s">
+      <c r="C103" s="33" t="s">
         <v>96</v>
       </c>
       <c r="D103" s="12"/>
@@ -5339,14 +5391,9 @@
       <c r="F103" s="11"/>
       <c r="G103" s="11"/>
       <c r="H103" s="13"/>
-      <c r="I103" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="J103" s="28"/>
-      <c r="K103" s="29" t="str">
-        <f t="shared" si="5"/>
-        <v>Version</v>
-      </c>
+      <c r="I103" s="27"/>
+      <c r="J103" s="27"/>
+      <c r="K103" s="28"/>
       <c r="L103" s="20" t="s">
         <v>214</v>
       </c>
@@ -5358,7 +5405,7 @@
       <c r="B104" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C104" s="50" t="s">
+      <c r="C104" s="34" t="s">
         <v>303</v>
       </c>
       <c r="D104" s="12"/>
@@ -5366,22 +5413,9 @@
       <c r="F104" s="11"/>
       <c r="G104" s="11"/>
       <c r="H104" s="13"/>
-      <c r="I104" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="J104" s="28"/>
-      <c r="K104" s="29" t="str">
-        <f t="shared" si="5"/>
-        <v>[h1]Description[/h1]
-Ce mod force les prisonniers à travailler. Pour activer cette fonctionnalité, les prisonniers doivent avoir l’option « Forcer à travailler » de coché dans l’onglet « Prisonnier ». Prison labor nécessite une gestion qui consiste en :
-[list]
-[*] Motivation – les prisonniers doivent êtres motivés par la présence de colons. Les gardiens ont un nouveau travail – superviser les prisonniers.Une faible motivation peut mener à des révoltes.
-[*] Assignation du travail – les prisonniers qui ont l’option « Forcer à travailler » cochée seront ajoutés à l’onglet « Travail ».
-[*] Restriction du temps - les prisonniers qui ont l’option « Forcer à travailler » cochée seront ajoutés à l’onglet «Restriction».
-[*] Zone de prison -pour travailler, un prisonnier doit avoir un chemin d’accès à son travail.Vous pouvez coché l’option « maintenir ouvert » sur des portes pour laisser un passage. Soyez prudents, ils essayeront de s’échapper si ils en ont l’opportunité.
-[*] L’outil « Prisonnier seulement » -Vous pouvez marquer des ordres par cet outil, ce qui exclu les colons pour ce travail
-[/list]</v>
-      </c>
+      <c r="I104" s="27"/>
+      <c r="J104" s="27"/>
+      <c r="K104" s="28"/>
       <c r="L104" s="20" t="s">
         <v>214</v>
       </c>
@@ -5393,7 +5427,7 @@
       <c r="B105" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C105" s="50" t="s">
+      <c r="C105" s="34" t="s">
         <v>304</v>
       </c>
       <c r="D105" s="12"/>
@@ -5401,15 +5435,9 @@
       <c r="F105" s="11"/>
       <c r="G105" s="11"/>
       <c r="H105" s="13"/>
-      <c r="I105" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="J105" s="28"/>
-      <c r="K105" s="29" t="str">
-        <f t="shared" si="5"/>
-        <v>[h1]Beta note[/h1]
-Ceci est une version Beta. Certains aspects du mod peuvent toujours être rééquilibrés  (comme la motivation). Il peut également y avoir quelques bugs.</v>
-      </c>
+      <c r="I105" s="27"/>
+      <c r="J105" s="27"/>
+      <c r="K105" s="28"/>
       <c r="L105" s="20" t="s">
         <v>214</v>
       </c>
@@ -5421,7 +5449,7 @@
       <c r="B106" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C106" s="50" t="s">
+      <c r="C106" s="34" t="s">
         <v>99</v>
       </c>
       <c r="D106" s="12"/>
@@ -5429,17 +5457,9 @@
       <c r="F106" s="11"/>
       <c r="G106" s="11"/>
       <c r="H106" s="13"/>
-      <c r="I106" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="J106" s="28"/>
-      <c r="K106" s="29" t="str">
-        <f t="shared" si="5"/>
-        <v>[h1]Links[/h1]
-[url=]Download[/url]
-[url=]Github[/url]
-[url=]Credits[/url]</v>
-      </c>
+      <c r="I106" s="27"/>
+      <c r="J106" s="27"/>
+      <c r="K106" s="28"/>
       <c r="L106" s="20" t="s">
         <v>214</v>
       </c>
@@ -5451,7 +5471,7 @@
       <c r="B107" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C107" s="50" t="s">
+      <c r="C107" s="34" t="s">
         <v>305</v>
       </c>
       <c r="D107" s="12"/>
@@ -5459,15 +5479,9 @@
       <c r="F107" s="11"/>
       <c r="G107" s="11"/>
       <c r="H107" s="14"/>
-      <c r="I107" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="J107" s="30"/>
-      <c r="K107" s="26" t="str">
-        <f t="shared" si="5"/>
-        <v>[h1]Locks mod (mod verrou)[/h1]
-Je recommande fortement d’utiliser mon autre mod [url=http://steamcommunity.com/sharedfiles/filedetails/?id=1157085076]Locks[/url]. Cela vous permettra d’autoriser les prisonniers à franchir certaines portes.</v>
-      </c>
+      <c r="I107" s="29"/>
+      <c r="J107" s="29"/>
+      <c r="K107" s="26"/>
       <c r="L107" s="20" t="s">
         <v>214</v>
       </c>

</xml_diff>